<commit_message>
Denote DestinationETA on Collections as Optional
</commit_message>
<xml_diff>
--- a/Schema/ERMSchemaDoc.xlsx
+++ b/Schema/ERMSchemaDoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_code\enterprise-route-management\Schema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mich4255/Documents/_products/ERM/schema/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A3961C-2ED6-4E4B-BC8C-62BF073910ED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9205334E-201D-754D-8869-8E076B74341B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{EDA34701-FAC7-4199-B2BF-D142CEC30FB3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{EDA34701-FAC7-4199-B2BF-D142CEC30FB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema-AllClasses" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2027,24 +2029,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32153D81-AD30-43DC-A256-1E031514BB29}">
   <dimension ref="A1:H277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H94" sqref="H94"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B237" sqref="B237"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="29.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" style="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" style="1"/>
+    <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" customWidth="1"/>
-    <col min="7" max="7" width="43.7109375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="43.6640625" style="10" customWidth="1"/>
     <col min="8" max="8" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -2070,7 +2072,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -2095,7 +2097,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -2120,7 +2122,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
@@ -2139,7 +2141,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -2164,7 +2166,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -2189,7 +2191,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -2214,7 +2216,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -2239,7 +2241,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -2264,7 +2266,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -2289,7 +2291,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
@@ -2308,7 +2310,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
@@ -2327,7 +2329,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2346,7 +2348,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
@@ -2365,7 +2367,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
@@ -2384,7 +2386,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2408,7 +2410,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -2432,7 +2434,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -2456,7 +2458,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -2480,7 +2482,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -2505,7 +2507,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -2532,7 +2534,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D22" s="2"/>
       <c r="E22" s="4" t="b">
         <f t="shared" ref="E22:E85" si="1">OR(ISBLANK(B22),ISBLANK(D22),B22=D22,D22="*not currently supported*")</f>
@@ -2540,7 +2542,7 @@
       </c>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>46</v>
       </c>
@@ -2562,7 +2564,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -2584,7 +2586,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -2609,7 +2611,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>46</v>
       </c>
@@ -2634,7 +2636,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="C27" s="1" t="s">
         <v>179</v>
       </c>
@@ -2653,7 +2655,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="C28" s="1" t="s">
         <v>179</v>
       </c>
@@ -2672,7 +2674,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C29" s="1" t="s">
         <v>179</v>
       </c>
@@ -2691,7 +2693,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C30" s="1" t="s">
         <v>179</v>
       </c>
@@ -2710,7 +2712,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
         <v>179</v>
       </c>
@@ -2726,7 +2728,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>46</v>
       </c>
@@ -2751,7 +2753,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>46</v>
       </c>
@@ -2776,7 +2778,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -2801,7 +2803,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>46</v>
       </c>
@@ -2826,7 +2828,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>46</v>
       </c>
@@ -2851,7 +2853,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
@@ -2876,7 +2878,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>46</v>
       </c>
@@ -2895,7 +2897,7 @@
       </c>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
@@ -2920,7 +2922,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>46</v>
       </c>
@@ -2945,7 +2947,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>46</v>
       </c>
@@ -2970,7 +2972,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="112" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
@@ -2992,7 +2994,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>46</v>
       </c>
@@ -3017,7 +3019,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>46</v>
       </c>
@@ -3042,7 +3044,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A45" s="13" t="s">
         <v>46</v>
       </c>
@@ -3067,7 +3069,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
@@ -3092,7 +3094,7 @@
       </c>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -3117,7 +3119,7 @@
       </c>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -3142,7 +3144,7 @@
       </c>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>46</v>
       </c>
@@ -3167,7 +3169,7 @@
       </c>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C50" s="1" t="s">
         <v>179</v>
       </c>
@@ -3186,7 +3188,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C51" s="1" t="s">
         <v>179</v>
       </c>
@@ -3205,7 +3207,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C52" s="1" t="s">
         <v>179</v>
       </c>
@@ -3224,7 +3226,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C53" s="1" t="s">
         <v>179</v>
       </c>
@@ -3243,7 +3245,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C54" s="1" t="s">
         <v>179</v>
       </c>
@@ -3262,7 +3264,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>46</v>
       </c>
@@ -3287,7 +3289,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>46</v>
       </c>
@@ -3314,7 +3316,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>46</v>
       </c>
@@ -3341,7 +3343,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>46</v>
       </c>
@@ -3363,7 +3365,7 @@
       </c>
       <c r="H58" s="1"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>46</v>
       </c>
@@ -3387,7 +3389,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>46</v>
       </c>
@@ -3414,7 +3416,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>46</v>
       </c>
@@ -3441,7 +3443,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="C62" s="1" t="s">
         <v>179</v>
       </c>
@@ -3462,7 +3464,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="C63" s="1" t="s">
         <v>179</v>
       </c>
@@ -3483,7 +3485,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="C64" s="1" t="s">
         <v>179</v>
       </c>
@@ -3504,7 +3506,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>46</v>
       </c>
@@ -3529,7 +3531,7 @@
       </c>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>46</v>
       </c>
@@ -3554,7 +3556,7 @@
       </c>
       <c r="H66" s="1"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>46</v>
       </c>
@@ -3571,7 +3573,7 @@
       <c r="F67" s="6"/>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>46</v>
       </c>
@@ -3587,7 +3589,7 @@
       </c>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>46</v>
       </c>
@@ -3614,7 +3616,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>46</v>
       </c>
@@ -3633,7 +3635,7 @@
       </c>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>46</v>
       </c>
@@ -3660,7 +3662,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>46</v>
       </c>
@@ -3687,7 +3689,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D73" s="2" t="s">
         <v>199</v>
       </c>
@@ -3699,7 +3701,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D74" s="2" t="s">
         <v>199</v>
       </c>
@@ -3711,7 +3713,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C75" s="1" t="s">
         <v>179</v>
       </c>
@@ -3729,7 +3731,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C76" s="1" t="s">
         <v>179</v>
       </c>
@@ -3747,7 +3749,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C77" s="1" t="s">
         <v>179</v>
       </c>
@@ -3765,7 +3767,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C78" s="1" t="s">
         <v>179</v>
       </c>
@@ -3783,7 +3785,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C79" s="1" t="s">
         <v>179</v>
       </c>
@@ -3801,7 +3803,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C80" s="1" t="s">
         <v>179</v>
       </c>
@@ -3819,7 +3821,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C81" s="1" t="s">
         <v>179</v>
       </c>
@@ -3837,7 +3839,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C82" s="1" t="s">
         <v>179</v>
       </c>
@@ -3855,7 +3857,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C83" s="1" t="s">
         <v>179</v>
       </c>
@@ -3873,7 +3875,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C84" s="1" t="s">
         <v>179</v>
       </c>
@@ -3885,7 +3887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C85" s="1" t="s">
         <v>179</v>
       </c>
@@ -3897,7 +3899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C86" s="1" t="s">
         <v>179</v>
       </c>
@@ -3915,7 +3917,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C87" s="1" t="s">
         <v>179</v>
       </c>
@@ -3933,7 +3935,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C88" s="1" t="s">
         <v>179</v>
       </c>
@@ -3951,7 +3953,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C89" s="1" t="s">
         <v>179</v>
       </c>
@@ -3969,7 +3971,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C90" s="1" t="s">
         <v>179</v>
       </c>
@@ -3987,7 +3989,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C91" s="1" t="s">
         <v>179</v>
       </c>
@@ -4002,7 +4004,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C92" s="1" t="s">
         <v>179</v>
       </c>
@@ -4017,7 +4019,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C93" s="1" t="s">
         <v>179</v>
       </c>
@@ -4032,7 +4034,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>87</v>
       </c>
@@ -4053,7 +4055,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>87</v>
       </c>
@@ -4074,7 +4076,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>87</v>
       </c>
@@ -4098,7 +4100,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="B97" s="1" t="s">
         <v>2</v>
       </c>
@@ -4119,7 +4121,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>87</v>
       </c>
@@ -4143,7 +4145,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>87</v>
       </c>
@@ -4167,7 +4169,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C100" s="1" t="s">
         <v>195</v>
       </c>
@@ -4182,7 +4184,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C101" s="1" t="s">
         <v>195</v>
       </c>
@@ -4197,7 +4199,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>87</v>
       </c>
@@ -4221,7 +4223,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>87</v>
       </c>
@@ -4245,7 +4247,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>87</v>
       </c>
@@ -4269,7 +4271,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>87</v>
       </c>
@@ -4293,7 +4295,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>87</v>
       </c>
@@ -4317,7 +4319,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>87</v>
       </c>
@@ -4344,7 +4346,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>87</v>
       </c>
@@ -4368,7 +4370,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>87</v>
       </c>
@@ -4392,7 +4394,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>87</v>
       </c>
@@ -4416,7 +4418,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>87</v>
       </c>
@@ -4440,7 +4442,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>87</v>
       </c>
@@ -4464,7 +4466,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="C113" s="1" t="s">
         <v>195</v>
       </c>
@@ -4482,7 +4484,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="C114" s="1" t="s">
         <v>195</v>
       </c>
@@ -4500,7 +4502,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="C115" s="1" t="s">
         <v>195</v>
       </c>
@@ -4518,7 +4520,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C116" s="1" t="s">
         <v>195</v>
       </c>
@@ -4536,7 +4538,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C117" s="1" t="s">
         <v>195</v>
       </c>
@@ -4554,7 +4556,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>87</v>
       </c>
@@ -4578,7 +4580,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>87</v>
       </c>
@@ -4602,7 +4604,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>87</v>
       </c>
@@ -4626,7 +4628,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>87</v>
       </c>
@@ -4650,7 +4652,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>87</v>
       </c>
@@ -4674,7 +4676,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>87</v>
       </c>
@@ -4698,7 +4700,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>87</v>
       </c>
@@ -4722,7 +4724,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>87</v>
       </c>
@@ -4749,7 +4751,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>87</v>
       </c>
@@ -4776,7 +4778,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>87</v>
       </c>
@@ -4803,7 +4805,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>87</v>
       </c>
@@ -4830,7 +4832,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>87</v>
       </c>
@@ -4857,7 +4859,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>87</v>
       </c>
@@ -4884,7 +4886,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>87</v>
       </c>
@@ -4911,7 +4913,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>87</v>
       </c>
@@ -4938,7 +4940,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>87</v>
       </c>
@@ -4965,7 +4967,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>87</v>
       </c>
@@ -4992,7 +4994,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>87</v>
       </c>
@@ -5019,7 +5021,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>87</v>
       </c>
@@ -5037,7 +5039,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>87</v>
       </c>
@@ -5055,7 +5057,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>87</v>
       </c>
@@ -5082,7 +5084,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>87</v>
       </c>
@@ -5109,7 +5111,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>87</v>
       </c>
@@ -5136,7 +5138,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>87</v>
       </c>
@@ -5163,7 +5165,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>87</v>
       </c>
@@ -5190,7 +5192,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>87</v>
       </c>
@@ -5217,7 +5219,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C144" s="1" t="s">
         <v>195</v>
       </c>
@@ -5235,7 +5237,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C145" s="1" t="s">
         <v>195</v>
       </c>
@@ -5253,7 +5255,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C146" s="1" t="s">
         <v>195</v>
       </c>
@@ -5271,7 +5273,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C147" s="1" t="s">
         <v>195</v>
       </c>
@@ -5289,7 +5291,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C148" s="1" t="s">
         <v>195</v>
       </c>
@@ -5307,7 +5309,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C149" s="1" t="s">
         <v>195</v>
       </c>
@@ -5322,7 +5324,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C150" s="1" t="s">
         <v>195</v>
       </c>
@@ -5337,7 +5339,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C151" s="1" t="s">
         <v>195</v>
       </c>
@@ -5352,7 +5354,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C152" s="1" t="s">
         <v>195</v>
       </c>
@@ -5367,7 +5369,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C153" s="1" t="s">
         <v>195</v>
       </c>
@@ -5382,7 +5384,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C154" s="1" t="s">
         <v>195</v>
       </c>
@@ -5397,7 +5399,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C155" s="1" t="s">
         <v>195</v>
       </c>
@@ -5412,7 +5414,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>97</v>
       </c>
@@ -5433,7 +5435,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>97</v>
       </c>
@@ -5457,7 +5459,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>97</v>
       </c>
@@ -5484,7 +5486,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>97</v>
       </c>
@@ -5511,7 +5513,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>97</v>
       </c>
@@ -5538,7 +5540,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>97</v>
       </c>
@@ -5560,7 +5562,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>97</v>
       </c>
@@ -5582,7 +5584,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>97</v>
       </c>
@@ -5606,7 +5608,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>97</v>
       </c>
@@ -5630,7 +5632,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>97</v>
       </c>
@@ -5652,7 +5654,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>97</v>
       </c>
@@ -5674,7 +5676,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>97</v>
       </c>
@@ -5696,7 +5698,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>97</v>
       </c>
@@ -5715,7 +5717,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>97</v>
       </c>
@@ -5734,7 +5736,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>97</v>
       </c>
@@ -5758,7 +5760,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>97</v>
       </c>
@@ -5782,7 +5784,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>97</v>
       </c>
@@ -5803,7 +5805,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>97</v>
       </c>
@@ -5824,7 +5826,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>97</v>
       </c>
@@ -5845,7 +5847,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>97</v>
       </c>
@@ -5866,7 +5868,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>97</v>
       </c>
@@ -5887,7 +5889,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C177" s="1" t="s">
         <v>134</v>
       </c>
@@ -5902,7 +5904,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C178" s="1" t="s">
         <v>134</v>
       </c>
@@ -5917,7 +5919,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C179" s="1" t="s">
         <v>134</v>
       </c>
@@ -5932,7 +5934,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C180" s="1" t="s">
         <v>134</v>
       </c>
@@ -5947,7 +5949,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>95</v>
       </c>
@@ -5968,7 +5970,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>95</v>
       </c>
@@ -5992,7 +5994,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>95</v>
       </c>
@@ -6016,7 +6018,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>95</v>
       </c>
@@ -6040,7 +6042,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>95</v>
       </c>
@@ -6064,7 +6066,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>95</v>
       </c>
@@ -6088,7 +6090,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C187" s="1" t="s">
         <v>196</v>
       </c>
@@ -6103,7 +6105,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>95</v>
       </c>
@@ -6127,7 +6129,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>95</v>
       </c>
@@ -6151,7 +6153,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>95</v>
       </c>
@@ -6175,7 +6177,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>95</v>
       </c>
@@ -6199,7 +6201,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="192" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>95</v>
       </c>
@@ -6223,7 +6225,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
         <v>95</v>
       </c>
@@ -6247,7 +6249,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="194" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
         <v>95</v>
       </c>
@@ -6271,7 +6273,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
         <v>95</v>
       </c>
@@ -6295,7 +6297,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>95</v>
       </c>
@@ -6319,7 +6321,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>95</v>
       </c>
@@ -6343,7 +6345,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="198" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
         <v>95</v>
       </c>
@@ -6367,7 +6369,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>95</v>
       </c>
@@ -6382,7 +6384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>95</v>
       </c>
@@ -6397,7 +6399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>95</v>
       </c>
@@ -6421,7 +6423,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>95</v>
       </c>
@@ -6445,7 +6447,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="203" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>95</v>
       </c>
@@ -6469,7 +6471,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>95</v>
       </c>
@@ -6493,7 +6495,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="205" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
         <v>95</v>
       </c>
@@ -6517,7 +6519,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
         <v>95</v>
       </c>
@@ -6541,7 +6543,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C207" s="1" t="s">
         <v>196</v>
       </c>
@@ -6556,7 +6558,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C208" s="1" t="s">
         <v>196</v>
       </c>
@@ -6571,7 +6573,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C209" s="1" t="s">
         <v>196</v>
       </c>
@@ -6586,7 +6588,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C210" s="1" t="s">
         <v>196</v>
       </c>
@@ -6601,7 +6603,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>99</v>
       </c>
@@ -6622,7 +6624,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
         <v>99</v>
       </c>
@@ -6643,7 +6645,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="213" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
         <v>99</v>
       </c>
@@ -6664,7 +6666,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>99</v>
       </c>
@@ -6688,7 +6690,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C215" s="1" t="s">
         <v>197</v>
       </c>
@@ -6703,7 +6705,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C216" s="1" t="s">
         <v>197</v>
       </c>
@@ -6718,7 +6720,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C217" s="1" t="s">
         <v>197</v>
       </c>
@@ -6733,7 +6735,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C218" s="1" t="s">
         <v>197</v>
       </c>
@@ -6748,7 +6750,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C219" s="1" t="s">
         <v>197</v>
       </c>
@@ -6763,7 +6765,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="220" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A220" s="1" t="s">
         <v>101</v>
       </c>
@@ -6781,7 +6783,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="221" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>101</v>
       </c>
@@ -6799,7 +6801,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="222" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A222" s="1" t="s">
         <v>101</v>
       </c>
@@ -6817,7 +6819,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="223" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>101</v>
       </c>
@@ -6835,7 +6837,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="224" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A224" s="1" t="s">
         <v>101</v>
       </c>
@@ -6853,7 +6855,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>102</v>
       </c>
@@ -6874,7 +6876,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="226" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>102</v>
       </c>
@@ -6898,7 +6900,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>102</v>
       </c>
@@ -6916,7 +6918,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D228" s="1" t="s">
         <v>191</v>
       </c>
@@ -6928,7 +6930,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D229" s="1" t="s">
         <v>192</v>
       </c>
@@ -6940,7 +6942,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D230" s="1" t="s">
         <v>193</v>
       </c>
@@ -6952,7 +6954,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="D231" s="1" t="s">
         <v>194</v>
       </c>
@@ -6964,7 +6966,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>103</v>
       </c>
@@ -6985,7 +6987,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>103</v>
       </c>
@@ -7009,7 +7011,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>103</v>
       </c>
@@ -7033,7 +7035,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>103</v>
       </c>
@@ -7057,7 +7059,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C238" s="1" t="s">
         <v>338</v>
       </c>
@@ -7071,7 +7073,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C239" s="1" t="s">
         <v>338</v>
       </c>
@@ -7085,7 +7087,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C240" s="1" t="s">
         <v>338</v>
       </c>
@@ -7096,10 +7098,10 @@
         <v>429</v>
       </c>
       <c r="H240" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="241" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="241" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C241" s="1" t="s">
         <v>338</v>
       </c>
@@ -7113,7 +7115,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="242" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C242" s="1" t="s">
         <v>338</v>
       </c>
@@ -7127,7 +7129,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="243" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="243" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C243" s="1" t="s">
         <v>338</v>
       </c>
@@ -7141,7 +7143,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="244" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="244" spans="3:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C244" s="1" t="s">
         <v>338</v>
       </c>
@@ -7155,7 +7157,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="245" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C245" s="1" t="s">
         <v>338</v>
       </c>
@@ -7169,7 +7171,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="246" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="246" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C246" s="1" t="s">
         <v>338</v>
       </c>
@@ -7183,7 +7185,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="247" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="247" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C247" s="1" t="s">
         <v>338</v>
       </c>
@@ -7197,7 +7199,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="248" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="248" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C248" s="1" t="s">
         <v>338</v>
       </c>
@@ -7211,7 +7213,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="249" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C249" s="1" t="s">
         <v>338</v>
       </c>
@@ -7225,7 +7227,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="250" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C250" s="1" t="s">
         <v>338</v>
       </c>
@@ -7237,7 +7239,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="251" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C251" s="1" t="s">
         <v>338</v>
       </c>
@@ -7249,7 +7251,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="252" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C252" s="1" t="s">
         <v>338</v>
       </c>
@@ -7261,7 +7263,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="253" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C253" s="1" t="s">
         <v>338</v>
       </c>
@@ -7273,7 +7275,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="255" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C255" s="1" t="s">
         <v>433</v>
       </c>
@@ -7281,7 +7283,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="256" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C256" s="1" t="s">
         <v>433</v>
       </c>
@@ -7292,7 +7294,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="257" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C257" s="1" t="s">
         <v>433</v>
       </c>
@@ -7306,7 +7308,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="258" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C258" s="1" t="s">
         <v>433</v>
       </c>
@@ -7320,7 +7322,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="259" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C259" s="1" t="s">
         <v>433</v>
       </c>
@@ -7334,7 +7336,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="260" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C260" s="1" t="s">
         <v>433</v>
       </c>
@@ -7345,7 +7347,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="261" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C261" s="1" t="s">
         <v>433</v>
       </c>
@@ -7359,7 +7361,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="262" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C262" s="1" t="s">
         <v>433</v>
       </c>
@@ -7373,7 +7375,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="263" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:8" ht="48" x14ac:dyDescent="0.2">
       <c r="C263" s="1" t="s">
         <v>433</v>
       </c>
@@ -7387,7 +7389,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="264" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C264" s="1" t="s">
         <v>433</v>
       </c>
@@ -7401,7 +7403,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="265" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:8" ht="32" x14ac:dyDescent="0.2">
       <c r="C265" s="1" t="s">
         <v>433</v>
       </c>
@@ -7415,7 +7417,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="266" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C266" s="1" t="s">
         <v>433</v>
       </c>
@@ -7429,7 +7431,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="267" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C267" s="1" t="s">
         <v>433</v>
       </c>
@@ -7443,7 +7445,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="268" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C268" s="1" t="s">
         <v>433</v>
       </c>
@@ -7454,7 +7456,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="269" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C269" s="1" t="s">
         <v>433</v>
       </c>
@@ -7468,7 +7470,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="270" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C270" s="1" t="s">
         <v>433</v>
       </c>
@@ -7482,7 +7484,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="271" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C271" s="1" t="s">
         <v>433</v>
       </c>
@@ -7496,7 +7498,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="272" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C272" s="1" t="s">
         <v>433</v>
       </c>
@@ -7510,7 +7512,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="273" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C273" s="1" t="s">
         <v>433</v>
       </c>
@@ -7524,7 +7526,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="274" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C274" s="1" t="s">
         <v>433</v>
       </c>
@@ -7535,7 +7537,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="275" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C275" s="1" t="s">
         <v>433</v>
       </c>
@@ -7546,7 +7548,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="276" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C276" s="1" t="s">
         <v>433</v>
       </c>
@@ -7557,7 +7559,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="277" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:8" ht="16" x14ac:dyDescent="0.2">
       <c r="C277" s="1" t="s">
         <v>433</v>
       </c>
@@ -7813,18 +7815,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7847,14 +7849,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D93A991-478B-499D-AF9B-1F0B37B6B22A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{961E40A6-F9B0-4484-A79E-BC0DB6B09F97}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -7869,4 +7863,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D93A991-478B-499D-AF9B-1F0B37B6B22A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>